<commit_message>
fix and add name mappings
</commit_message>
<xml_diff>
--- a/Records.xlsx
+++ b/Records.xlsx
@@ -14,12 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>29-12-2023</t>
   </si>
   <si>
+    <t>01-01-2024</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Не ответил</t>
+  </si>
+  <si>
+    <t>Почти выздоровел</t>
+  </si>
+  <si>
+    <t>Панченко Иван</t>
+  </si>
+  <si>
     <t>Болен</t>
+  </si>
+  <si>
+    <t>Здоров</t>
   </si>
 </sst>
 </file>
@@ -35,16 +53,34 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF62C6FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB762"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF62FF97"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -61,9 +97,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,23 +397,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>86213130</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>